<commit_message>
update raw backend with new data - we added 1-025
</commit_message>
<xml_diff>
--- a/data/raw/VCAS-rove_time.xlsx
+++ b/data/raw/VCAS-rove_time.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11207"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10402"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jonathansalas/R_Projects/VCAS1_prelim_efficiency/data/raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0B650C3-F5CC-D84A-AED5-D6D04C5E4849}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2037EBE0-374E-A440-AB81-C9B4ECBE26BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20060" activeTab="1" xr2:uid="{0490BC07-0248-8949-839E-74C08EF47166}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="34560" windowHeight="21600" firstSheet="11" activeTab="31" xr2:uid="{0490BC07-0248-8949-839E-74C08EF47166}"/>
   </bookViews>
   <sheets>
     <sheet name="Notes" sheetId="1" r:id="rId1"/>
@@ -43,6 +43,8 @@
     <sheet name="1-021" sheetId="36" r:id="rId28"/>
     <sheet name="1-022" sheetId="37" r:id="rId29"/>
     <sheet name="1-023" sheetId="38" r:id="rId30"/>
+    <sheet name="1-024" sheetId="39" r:id="rId31"/>
+    <sheet name="1-025" sheetId="40" r:id="rId32"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -101,7 +103,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="540" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="570" uniqueCount="170">
   <si>
     <t>Here we track total ablation time which I will refer to going forward as rove_time</t>
   </si>
@@ -699,6 +701,24 @@
   <si>
     <t>https://fieldmedical.sharepoint.com/:v:/r/sites/Clinical/Shared%20Documents/VCAS%20Study/TMF-%20Subject%20Files/1-023/Footage/mix.mp4?csf=1&amp;web=1&amp;e=KnIY90</t>
   </si>
+  <si>
+    <t>1-024</t>
+  </si>
+  <si>
+    <t>1-025</t>
+  </si>
+  <si>
+    <t>Puts the Octaray back there to update the impedance field</t>
+  </si>
+  <si>
+    <t>Stop for post abl remap 1</t>
+  </si>
+  <si>
+    <t>Targetting residual potentials after 1st remap</t>
+  </si>
+  <si>
+    <t>Done</t>
+  </si>
 </sst>
 </file>
 
@@ -861,7 +881,25 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="90">
+  <dxfs count="96">
+    <dxf>
+      <numFmt numFmtId="26" formatCode="hh:mm:ss"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="h:mm:ss;@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="h:mm:ss;@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="26" formatCode="hh:mm:ss"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="h:mm:ss;@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="h:mm:ss;@"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="26" formatCode="hh:mm:ss"/>
     </dxf>
@@ -1155,14 +1193,14 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{C55969D0-B28D-F248-8DCD-E81C0E8043BD}" name="Table1" displayName="Table1" ref="A1:G39" totalsRowShown="0">
   <autoFilter ref="A1:G39" xr:uid="{C55969D0-B28D-F248-8DCD-E81C0E8043BD}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{718012BD-7025-314F-8E4E-E629C18A0C65}" name="subjectId" dataDxfId="89"/>
-    <tableColumn id="2" xr3:uid="{461579DB-75ED-D945-B839-5CC1464620BE}" name="rove_time" dataDxfId="88"/>
-    <tableColumn id="8" xr3:uid="{5E0CEC32-C01F-A446-827E-6309FE417F82}" name="dwell_time" dataDxfId="87">
+    <tableColumn id="1" xr3:uid="{718012BD-7025-314F-8E4E-E629C18A0C65}" name="subjectId" dataDxfId="95"/>
+    <tableColumn id="2" xr3:uid="{461579DB-75ED-D945-B839-5CC1464620BE}" name="rove_time" dataDxfId="94"/>
+    <tableColumn id="8" xr3:uid="{5E0CEC32-C01F-A446-827E-6309FE417F82}" name="dwell_time" dataDxfId="93">
       <calculatedColumnFormula>'1-001'!H35</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{E391ECC4-3F7C-C84F-9F85-065534605FDC}" name="etiology" dataDxfId="86"/>
-    <tableColumn id="6" xr3:uid="{18DD3274-05B0-9245-BC8D-9610E146E79C}" name="therapy" dataDxfId="85"/>
-    <tableColumn id="4" xr3:uid="{3166333D-6394-D34A-93C0-598B4DEC56B1}" name="notes" dataDxfId="84"/>
+    <tableColumn id="9" xr3:uid="{E391ECC4-3F7C-C84F-9F85-065534605FDC}" name="etiology" dataDxfId="92"/>
+    <tableColumn id="6" xr3:uid="{18DD3274-05B0-9245-BC8D-9610E146E79C}" name="therapy" dataDxfId="91"/>
+    <tableColumn id="4" xr3:uid="{3166333D-6394-D34A-93C0-598B4DEC56B1}" name="notes" dataDxfId="90"/>
     <tableColumn id="3" xr3:uid="{A7F69E93-3952-2D4F-B01B-B9EB9DC3432C}" name="link_to_data"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1173,9 +1211,9 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{F5A4CEBC-9F74-3B4A-97EE-FBFC2B092D3F}" name="Table24812" displayName="Table24812" ref="A1:D31" totalsRowShown="0">
   <autoFilter ref="A1:D31" xr:uid="{7DCBAB66-89F8-6F47-8D64-FA0C26924201}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{6B6BD5F2-A455-4741-BE8B-EB4069C30402}" name="start_time" dataDxfId="65"/>
-    <tableColumn id="2" xr3:uid="{1A57601A-180E-3841-905B-984320643C2E}" name="end_time" dataDxfId="64"/>
-    <tableColumn id="3" xr3:uid="{00349B95-06C5-6347-9812-8CE148323ABF}" name="time_diff" dataDxfId="63">
+    <tableColumn id="1" xr3:uid="{6B6BD5F2-A455-4741-BE8B-EB4069C30402}" name="start_time" dataDxfId="71"/>
+    <tableColumn id="2" xr3:uid="{1A57601A-180E-3841-905B-984320643C2E}" name="end_time" dataDxfId="70"/>
+    <tableColumn id="3" xr3:uid="{00349B95-06C5-6347-9812-8CE148323ABF}" name="time_diff" dataDxfId="69">
       <calculatedColumnFormula>Table24812[[#This Row],[end_time]]-Table24812[[#This Row],[start_time]]</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="4" xr3:uid="{F0480389-BE2E-CA47-91C9-281947E722D0}" name="notes"/>
@@ -1188,9 +1226,9 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="24" xr:uid="{3F78E5F9-8FC7-1747-90FF-3E51FC67A570}" name="Table245153456" displayName="Table245153456" ref="A1:D31" totalsRowShown="0">
   <autoFilter ref="A1:D31" xr:uid="{1A93302E-8621-7D48-88F2-5AC51E7EA3A4}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{F488A4D9-2DF8-D244-AEBC-805EFBE08DF6}" name="start_time" dataDxfId="62"/>
-    <tableColumn id="2" xr3:uid="{ACA4FF7E-238C-8F45-9565-DAD7F42E73B8}" name="end_time" dataDxfId="61"/>
-    <tableColumn id="3" xr3:uid="{F6BC8755-5891-4645-8170-88F754E99AA6}" name="time_diff" dataDxfId="60">
+    <tableColumn id="1" xr3:uid="{F488A4D9-2DF8-D244-AEBC-805EFBE08DF6}" name="start_time" dataDxfId="68"/>
+    <tableColumn id="2" xr3:uid="{ACA4FF7E-238C-8F45-9565-DAD7F42E73B8}" name="end_time" dataDxfId="67"/>
+    <tableColumn id="3" xr3:uid="{F6BC8755-5891-4645-8170-88F754E99AA6}" name="time_diff" dataDxfId="66">
       <calculatedColumnFormula>Table245153456[[#This Row],[end_time]]-Table245153456[[#This Row],[start_time]]</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="4" xr3:uid="{675A7FCC-306A-304D-91DC-89128A249BDF}" name="notes"/>
@@ -1203,9 +1241,9 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="25" xr:uid="{23DABAA4-E878-7146-A7F3-85DD83F4C855}" name="Table24515345" displayName="Table24515345" ref="A1:D31" totalsRowShown="0">
   <autoFilter ref="A1:D31" xr:uid="{1A93302E-8621-7D48-88F2-5AC51E7EA3A4}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{EE8B83DD-E65E-C441-9E58-95C830211436}" name="start_time" dataDxfId="59"/>
-    <tableColumn id="2" xr3:uid="{F6B57195-8D07-9240-B4C7-E06E1251BBF4}" name="end_time" dataDxfId="58"/>
-    <tableColumn id="3" xr3:uid="{F39F83CF-BB22-E54A-87DA-A8A19D2D22EA}" name="time_diff" dataDxfId="57">
+    <tableColumn id="1" xr3:uid="{EE8B83DD-E65E-C441-9E58-95C830211436}" name="start_time" dataDxfId="65"/>
+    <tableColumn id="2" xr3:uid="{F6B57195-8D07-9240-B4C7-E06E1251BBF4}" name="end_time" dataDxfId="64"/>
+    <tableColumn id="3" xr3:uid="{F39F83CF-BB22-E54A-87DA-A8A19D2D22EA}" name="time_diff" dataDxfId="63">
       <calculatedColumnFormula>Table24515345[[#This Row],[end_time]]-Table24515345[[#This Row],[start_time]]</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="4" xr3:uid="{486CF052-5F91-344A-902D-F2CA7FB8D506}" name="notes"/>
@@ -1218,9 +1256,9 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="26" xr:uid="{F1C0DDBF-006F-FE45-828C-B8FDAB683C59}" name="Table2451534" displayName="Table2451534" ref="A1:D31" totalsRowShown="0">
   <autoFilter ref="A1:D31" xr:uid="{1A93302E-8621-7D48-88F2-5AC51E7EA3A4}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{AD2DB3ED-B602-8946-99FC-F31C04E30CB1}" name="start_time" dataDxfId="56"/>
-    <tableColumn id="2" xr3:uid="{60EB5449-1ABA-D24F-9AB7-DA92E3458840}" name="end_time" dataDxfId="55"/>
-    <tableColumn id="3" xr3:uid="{0A4C1CEB-45DC-BC4A-B70E-CFFE5BC5F5CD}" name="time_diff" dataDxfId="54">
+    <tableColumn id="1" xr3:uid="{AD2DB3ED-B602-8946-99FC-F31C04E30CB1}" name="start_time" dataDxfId="62"/>
+    <tableColumn id="2" xr3:uid="{60EB5449-1ABA-D24F-9AB7-DA92E3458840}" name="end_time" dataDxfId="61"/>
+    <tableColumn id="3" xr3:uid="{0A4C1CEB-45DC-BC4A-B70E-CFFE5BC5F5CD}" name="time_diff" dataDxfId="60">
       <calculatedColumnFormula>Table2451534[[#This Row],[end_time]]-Table2451534[[#This Row],[start_time]]</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="4" xr3:uid="{48442FEA-2429-4A47-8FCB-D99F912F4A8E}" name="notes"/>
@@ -1233,9 +1271,9 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="27" xr:uid="{2C87F7CC-7C0F-0642-8F9A-FE038CD3FF1B}" name="Table245153" displayName="Table245153" ref="A1:D31" totalsRowShown="0">
   <autoFilter ref="A1:D31" xr:uid="{1A93302E-8621-7D48-88F2-5AC51E7EA3A4}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{1AC28B04-A977-FD4B-B78A-9DCC5E7EB80F}" name="start_time" dataDxfId="53"/>
-    <tableColumn id="2" xr3:uid="{C3B83CA2-3C6D-EA4A-BA2E-70FD53E04984}" name="end_time" dataDxfId="52"/>
-    <tableColumn id="3" xr3:uid="{4F86D6E1-1D92-8341-A9E9-53EB64E4C5D3}" name="time_diff" dataDxfId="51">
+    <tableColumn id="1" xr3:uid="{1AC28B04-A977-FD4B-B78A-9DCC5E7EB80F}" name="start_time" dataDxfId="59"/>
+    <tableColumn id="2" xr3:uid="{C3B83CA2-3C6D-EA4A-BA2E-70FD53E04984}" name="end_time" dataDxfId="58"/>
+    <tableColumn id="3" xr3:uid="{4F86D6E1-1D92-8341-A9E9-53EB64E4C5D3}" name="time_diff" dataDxfId="57">
       <calculatedColumnFormula>Table245153[[#This Row],[end_time]]-Table245153[[#This Row],[start_time]]</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="4" xr3:uid="{04931610-B628-D646-9B41-7F657DD32595}" name="notes"/>
@@ -1248,9 +1286,9 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{772A68B7-3577-954E-96AB-3F9F135762FE}" name="Table248" displayName="Table248" ref="A1:D31" totalsRowShown="0">
   <autoFilter ref="A1:D31" xr:uid="{7DCBAB66-89F8-6F47-8D64-FA0C26924201}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{6C1948AC-21BF-BA4D-A66C-95CD6D282814}" name="start_time" dataDxfId="50"/>
-    <tableColumn id="2" xr3:uid="{FCE64BF5-4264-4C43-929C-08AD08C28E78}" name="end_time" dataDxfId="49"/>
-    <tableColumn id="3" xr3:uid="{53FD3C4C-5892-8C4A-80B1-B3228D1980FF}" name="time_diff" dataDxfId="48">
+    <tableColumn id="1" xr3:uid="{6C1948AC-21BF-BA4D-A66C-95CD6D282814}" name="start_time" dataDxfId="56"/>
+    <tableColumn id="2" xr3:uid="{FCE64BF5-4264-4C43-929C-08AD08C28E78}" name="end_time" dataDxfId="55"/>
+    <tableColumn id="3" xr3:uid="{53FD3C4C-5892-8C4A-80B1-B3228D1980FF}" name="time_diff" dataDxfId="54">
       <calculatedColumnFormula>Table248[[#This Row],[end_time]]-Table248[[#This Row],[start_time]]</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="4" xr3:uid="{F22060DE-01C3-9C4C-A473-BCE8D37580D6}" name="notes"/>
@@ -1263,9 +1301,9 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{D84B3EF0-7875-184B-870A-3642242A31F0}" name="Table2410" displayName="Table2410" ref="A1:D31" totalsRowShown="0">
   <autoFilter ref="A1:D31" xr:uid="{7DCBAB66-89F8-6F47-8D64-FA0C26924201}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{3577E981-DDE4-CC47-8395-6FEE5951473E}" name="start_time" dataDxfId="47"/>
-    <tableColumn id="2" xr3:uid="{14BD1FB2-4172-BE43-8B3C-F4348552D39D}" name="end_time" dataDxfId="46"/>
-    <tableColumn id="3" xr3:uid="{EA005961-FE83-1F48-8259-AAAD2071A3B1}" name="time_diff" dataDxfId="45">
+    <tableColumn id="1" xr3:uid="{3577E981-DDE4-CC47-8395-6FEE5951473E}" name="start_time" dataDxfId="53"/>
+    <tableColumn id="2" xr3:uid="{14BD1FB2-4172-BE43-8B3C-F4348552D39D}" name="end_time" dataDxfId="52"/>
+    <tableColumn id="3" xr3:uid="{EA005961-FE83-1F48-8259-AAAD2071A3B1}" name="time_diff" dataDxfId="51">
       <calculatedColumnFormula>Table2410[[#This Row],[end_time]]-Table2410[[#This Row],[start_time]]</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="4" xr3:uid="{7A57ED91-2446-8F4F-95C2-3088CD96BD62}" name="notes"/>
@@ -1278,9 +1316,9 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{0A3CEC53-F376-1D4D-846C-0F34B09239B4}" name="Table249" displayName="Table249" ref="A1:D31" totalsRowShown="0">
   <autoFilter ref="A1:D31" xr:uid="{7DCBAB66-89F8-6F47-8D64-FA0C26924201}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{49600F71-5258-BD4C-B040-17EFB93CC626}" name="start_time" dataDxfId="44"/>
-    <tableColumn id="2" xr3:uid="{BDE18332-AF9E-6E4E-B81F-9AB511ACDD6F}" name="end_time" dataDxfId="43"/>
-    <tableColumn id="3" xr3:uid="{8AAE5943-30E3-C746-AE58-07515593AE41}" name="time_diff" dataDxfId="42">
+    <tableColumn id="1" xr3:uid="{49600F71-5258-BD4C-B040-17EFB93CC626}" name="start_time" dataDxfId="50"/>
+    <tableColumn id="2" xr3:uid="{BDE18332-AF9E-6E4E-B81F-9AB511ACDD6F}" name="end_time" dataDxfId="49"/>
+    <tableColumn id="3" xr3:uid="{8AAE5943-30E3-C746-AE58-07515593AE41}" name="time_diff" dataDxfId="48">
       <calculatedColumnFormula>Table249[[#This Row],[end_time]]-Table249[[#This Row],[start_time]]</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="4" xr3:uid="{7880A518-97D3-0D44-977A-E75D9468AB4A}" name="notes"/>
@@ -1293,9 +1331,9 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{A7ADDBBE-0483-F84D-98C5-791E3CFC3CE4}" name="Table24511" displayName="Table24511" ref="A1:D31" totalsRowShown="0">
   <autoFilter ref="A1:D31" xr:uid="{7DCBAB66-89F8-6F47-8D64-FA0C26924201}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{26C8DC9E-AF52-B74F-997F-91F760434CC8}" name="start_time" dataDxfId="41"/>
-    <tableColumn id="2" xr3:uid="{6083687F-E3D1-0F47-90EE-749E4C68F9D7}" name="end_time" dataDxfId="40"/>
-    <tableColumn id="3" xr3:uid="{11F768A3-7132-674C-8E3C-457C09009AD5}" name="time_diff" dataDxfId="39">
+    <tableColumn id="1" xr3:uid="{26C8DC9E-AF52-B74F-997F-91F760434CC8}" name="start_time" dataDxfId="47"/>
+    <tableColumn id="2" xr3:uid="{6083687F-E3D1-0F47-90EE-749E4C68F9D7}" name="end_time" dataDxfId="46"/>
+    <tableColumn id="3" xr3:uid="{11F768A3-7132-674C-8E3C-457C09009AD5}" name="time_diff" dataDxfId="45">
       <calculatedColumnFormula>Table24511[[#This Row],[end_time]]-Table24511[[#This Row],[start_time]]</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="4" xr3:uid="{6BF25E36-BEFE-334C-B53B-9359DA68008A}" name="notes"/>
@@ -1308,9 +1346,9 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{039AD6AB-0126-1947-A333-DE36DDA0B7E4}" name="Table245" displayName="Table245" ref="A1:D31" totalsRowShown="0">
   <autoFilter ref="A1:D31" xr:uid="{7DCBAB66-89F8-6F47-8D64-FA0C26924201}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{8C37C915-F94A-5148-A3D1-EE8B899AF7F8}" name="start_time" dataDxfId="38"/>
-    <tableColumn id="2" xr3:uid="{B8735F0A-4AB0-C54D-85C0-1F0A63FA3498}" name="end_time" dataDxfId="37"/>
-    <tableColumn id="3" xr3:uid="{12E891A6-DF38-EE41-AC70-EAADDDA13272}" name="time_diff" dataDxfId="36">
+    <tableColumn id="1" xr3:uid="{8C37C915-F94A-5148-A3D1-EE8B899AF7F8}" name="start_time" dataDxfId="44"/>
+    <tableColumn id="2" xr3:uid="{B8735F0A-4AB0-C54D-85C0-1F0A63FA3498}" name="end_time" dataDxfId="43"/>
+    <tableColumn id="3" xr3:uid="{12E891A6-DF38-EE41-AC70-EAADDDA13272}" name="time_diff" dataDxfId="42">
       <calculatedColumnFormula>Table245[[#This Row],[end_time]]-Table245[[#This Row],[start_time]]</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="4" xr3:uid="{F8493A5C-0C25-FD45-A552-FE369F4F3DAD}" name="notes"/>
@@ -1323,9 +1361,9 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{1A93302E-8621-7D48-88F2-5AC51E7EA3A4}" name="Table24515" displayName="Table24515" ref="A1:D31" totalsRowShown="0">
   <autoFilter ref="A1:D31" xr:uid="{1A93302E-8621-7D48-88F2-5AC51E7EA3A4}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{4542A81A-297E-DB48-B049-9309ACD42F2B}" name="start_time" dataDxfId="83"/>
-    <tableColumn id="2" xr3:uid="{FC99294C-6B9C-9349-BAD2-0D219F840C1B}" name="end_time" dataDxfId="82"/>
-    <tableColumn id="3" xr3:uid="{DBC27D03-BB8D-904E-8022-8B6335C64879}" name="time_diff" dataDxfId="81">
+    <tableColumn id="1" xr3:uid="{4542A81A-297E-DB48-B049-9309ACD42F2B}" name="start_time" dataDxfId="89"/>
+    <tableColumn id="2" xr3:uid="{FC99294C-6B9C-9349-BAD2-0D219F840C1B}" name="end_time" dataDxfId="88"/>
+    <tableColumn id="3" xr3:uid="{DBC27D03-BB8D-904E-8022-8B6335C64879}" name="time_diff" dataDxfId="87">
       <calculatedColumnFormula>Table24515[[#This Row],[end_time]]-Table24515[[#This Row],[start_time]]</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="4" xr3:uid="{D5223D27-0D62-AC4C-857C-038DCA9594DB}" name="notes"/>
@@ -1338,9 +1376,9 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{1825D363-0D01-614F-8BB6-B82D0839B62E}" name="Table245154" displayName="Table245154" ref="A1:D31" totalsRowShown="0">
   <autoFilter ref="A1:D31" xr:uid="{1A93302E-8621-7D48-88F2-5AC51E7EA3A4}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{85D813AA-3E14-AA49-8764-1AFB1744F6CB}" name="start_time" dataDxfId="35"/>
-    <tableColumn id="2" xr3:uid="{6FA6C7C4-391C-734C-A912-3190038D77AB}" name="end_time" dataDxfId="34"/>
-    <tableColumn id="3" xr3:uid="{9C4583F8-953A-D04B-AA91-7D77A5FF66F0}" name="time_diff" dataDxfId="33">
+    <tableColumn id="1" xr3:uid="{85D813AA-3E14-AA49-8764-1AFB1744F6CB}" name="start_time" dataDxfId="41"/>
+    <tableColumn id="2" xr3:uid="{6FA6C7C4-391C-734C-A912-3190038D77AB}" name="end_time" dataDxfId="40"/>
+    <tableColumn id="3" xr3:uid="{9C4583F8-953A-D04B-AA91-7D77A5FF66F0}" name="time_diff" dataDxfId="39">
       <calculatedColumnFormula>Table245154[[#This Row],[end_time]]-Table245154[[#This Row],[start_time]]</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="4" xr3:uid="{23A25CAD-E05F-1648-AA7C-0B4BD9C1739D}" name="notes"/>
@@ -1353,9 +1391,9 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="15" xr:uid="{CE45E49D-73E4-8A4C-B1C1-A5F171222BA6}" name="Table24515416" displayName="Table24515416" ref="A1:D31" totalsRowShown="0">
   <autoFilter ref="A1:D31" xr:uid="{1A93302E-8621-7D48-88F2-5AC51E7EA3A4}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{31B61C1F-509B-C549-8AEF-DF0658F2B96B}" name="start_time" dataDxfId="32"/>
-    <tableColumn id="2" xr3:uid="{091F6D25-E362-ED42-9029-E0BCEEAEA850}" name="end_time" dataDxfId="31"/>
-    <tableColumn id="3" xr3:uid="{318940A5-8075-5D4C-BD68-125D391D783D}" name="time_diff" dataDxfId="30">
+    <tableColumn id="1" xr3:uid="{31B61C1F-509B-C549-8AEF-DF0658F2B96B}" name="start_time" dataDxfId="38"/>
+    <tableColumn id="2" xr3:uid="{091F6D25-E362-ED42-9029-E0BCEEAEA850}" name="end_time" dataDxfId="37"/>
+    <tableColumn id="3" xr3:uid="{318940A5-8075-5D4C-BD68-125D391D783D}" name="time_diff" dataDxfId="36">
       <calculatedColumnFormula>Table24515416[[#This Row],[end_time]]-Table24515416[[#This Row],[start_time]]</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="4" xr3:uid="{4ECB2A10-B67B-D84C-9D70-CB15A16921DE}" name="notes"/>
@@ -1368,9 +1406,9 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="19" xr:uid="{130F2C16-F9C9-CF46-A41B-03CB1D6467B4}" name="Table2451517181920" displayName="Table2451517181920" ref="A1:D31" totalsRowShown="0">
   <autoFilter ref="A1:D31" xr:uid="{1A93302E-8621-7D48-88F2-5AC51E7EA3A4}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{58637CDA-F3F8-FB4F-825C-C88AA91FAD7B}" name="start_time" dataDxfId="29"/>
-    <tableColumn id="2" xr3:uid="{1096A82C-CDE7-4340-BAF9-3BAA3098CA7F}" name="end_time" dataDxfId="28"/>
-    <tableColumn id="3" xr3:uid="{02C5EC47-6504-E246-90FC-F20CBBDEB705}" name="time_diff" dataDxfId="27">
+    <tableColumn id="1" xr3:uid="{58637CDA-F3F8-FB4F-825C-C88AA91FAD7B}" name="start_time" dataDxfId="35"/>
+    <tableColumn id="2" xr3:uid="{1096A82C-CDE7-4340-BAF9-3BAA3098CA7F}" name="end_time" dataDxfId="34"/>
+    <tableColumn id="3" xr3:uid="{02C5EC47-6504-E246-90FC-F20CBBDEB705}" name="time_diff" dataDxfId="33">
       <calculatedColumnFormula>Table2451517181920[[#This Row],[end_time]]-Table2451517181920[[#This Row],[start_time]]</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="4" xr3:uid="{1469F086-E8DD-C741-AA69-4E9161FE65C0}" name="notes"/>
@@ -1383,9 +1421,9 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="18" xr:uid="{1029D1F1-1F5A-3E49-AF78-3C0DC1D2F68D}" name="Table24515171819" displayName="Table24515171819" ref="A1:D31" totalsRowShown="0">
   <autoFilter ref="A1:D31" xr:uid="{1A93302E-8621-7D48-88F2-5AC51E7EA3A4}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{044D31B5-AD7A-E643-B833-0826FB3FF28C}" name="start_time" dataDxfId="26"/>
-    <tableColumn id="2" xr3:uid="{65F326FC-ED53-1A4C-B3DE-07B092115C14}" name="end_time" dataDxfId="25"/>
-    <tableColumn id="3" xr3:uid="{FC649FAA-6E56-154B-8877-A16770D51793}" name="time_diff" dataDxfId="24">
+    <tableColumn id="1" xr3:uid="{044D31B5-AD7A-E643-B833-0826FB3FF28C}" name="start_time" dataDxfId="32"/>
+    <tableColumn id="2" xr3:uid="{65F326FC-ED53-1A4C-B3DE-07B092115C14}" name="end_time" dataDxfId="31"/>
+    <tableColumn id="3" xr3:uid="{FC649FAA-6E56-154B-8877-A16770D51793}" name="time_diff" dataDxfId="30">
       <calculatedColumnFormula>Table24515171819[[#This Row],[end_time]]-Table24515171819[[#This Row],[start_time]]</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="4" xr3:uid="{C770E668-C460-4649-98CE-000E807A6F4C}" name="notes"/>
@@ -1398,9 +1436,9 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="17" xr:uid="{A8099601-2538-9E41-BA1B-CA228C6B7FD8}" name="Table245151718" displayName="Table245151718" ref="A1:D31" totalsRowShown="0">
   <autoFilter ref="A1:D31" xr:uid="{1A93302E-8621-7D48-88F2-5AC51E7EA3A4}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{152C5995-5BCE-0F4A-AB21-E37E5A45CC96}" name="start_time" dataDxfId="23"/>
-    <tableColumn id="2" xr3:uid="{A314440D-1DAD-F747-8091-26BF031D535E}" name="end_time" dataDxfId="22"/>
-    <tableColumn id="3" xr3:uid="{8038CAE0-AE64-A94A-8EEC-196F11CC42FB}" name="time_diff" dataDxfId="21">
+    <tableColumn id="1" xr3:uid="{152C5995-5BCE-0F4A-AB21-E37E5A45CC96}" name="start_time" dataDxfId="29"/>
+    <tableColumn id="2" xr3:uid="{A314440D-1DAD-F747-8091-26BF031D535E}" name="end_time" dataDxfId="28"/>
+    <tableColumn id="3" xr3:uid="{8038CAE0-AE64-A94A-8EEC-196F11CC42FB}" name="time_diff" dataDxfId="27">
       <calculatedColumnFormula>Table245151718[[#This Row],[end_time]]-Table245151718[[#This Row],[start_time]]</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="4" xr3:uid="{E78FDFD8-421B-4B42-8E66-304EDA7C4631}" name="notes"/>
@@ -1413,9 +1451,9 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="16" xr:uid="{10879581-5376-9648-90EC-5599AE274B37}" name="Table2451517" displayName="Table2451517" ref="A1:D31" totalsRowShown="0">
   <autoFilter ref="A1:D31" xr:uid="{1A93302E-8621-7D48-88F2-5AC51E7EA3A4}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{2036FDA6-A87D-5C41-84BB-E2DE3418E515}" name="start_time" dataDxfId="20"/>
-    <tableColumn id="2" xr3:uid="{63FAF62F-E02F-9344-92DD-A7835371FD15}" name="end_time" dataDxfId="19"/>
-    <tableColumn id="3" xr3:uid="{84451293-C537-C74D-85BC-080896072B82}" name="time_diff" dataDxfId="18">
+    <tableColumn id="1" xr3:uid="{2036FDA6-A87D-5C41-84BB-E2DE3418E515}" name="start_time" dataDxfId="26"/>
+    <tableColumn id="2" xr3:uid="{63FAF62F-E02F-9344-92DD-A7835371FD15}" name="end_time" dataDxfId="25"/>
+    <tableColumn id="3" xr3:uid="{84451293-C537-C74D-85BC-080896072B82}" name="time_diff" dataDxfId="24">
       <calculatedColumnFormula>Table2451517[[#This Row],[end_time]]-Table2451517[[#This Row],[start_time]]</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="4" xr3:uid="{D9D1EDB1-9623-3A44-A4BF-E8857517A4BE}" name="notes"/>
@@ -1428,9 +1466,9 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="20" xr:uid="{2B4E61D6-F073-DC43-BDFC-32D5D661417D}" name="Table2451521" displayName="Table2451521" ref="A1:D31" totalsRowShown="0">
   <autoFilter ref="A1:D31" xr:uid="{1A93302E-8621-7D48-88F2-5AC51E7EA3A4}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{DBDC0137-E30C-354A-87F0-8FC256EE47DD}" name="start_time" dataDxfId="17"/>
-    <tableColumn id="2" xr3:uid="{F3C9949C-5E56-3043-B895-7F1C223F084C}" name="end_time" dataDxfId="16"/>
-    <tableColumn id="3" xr3:uid="{284C38E6-8B60-FF42-B36D-752AB81A0D3E}" name="time_diff" dataDxfId="15">
+    <tableColumn id="1" xr3:uid="{DBDC0137-E30C-354A-87F0-8FC256EE47DD}" name="start_time" dataDxfId="23"/>
+    <tableColumn id="2" xr3:uid="{F3C9949C-5E56-3043-B895-7F1C223F084C}" name="end_time" dataDxfId="22"/>
+    <tableColumn id="3" xr3:uid="{284C38E6-8B60-FF42-B36D-752AB81A0D3E}" name="time_diff" dataDxfId="21">
       <calculatedColumnFormula>Table2451521[[#This Row],[end_time]]-Table2451521[[#This Row],[start_time]]</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="4" xr3:uid="{997FD67A-B2F8-4047-8AFA-B14BF2F18FC2}" name="notes"/>
@@ -1443,9 +1481,9 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="21" xr:uid="{BA39C582-8A3B-4040-B00B-B16288D1ADEA}" name="Table245152122" displayName="Table245152122" ref="A1:D31" totalsRowShown="0">
   <autoFilter ref="A1:D31" xr:uid="{1A93302E-8621-7D48-88F2-5AC51E7EA3A4}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{25E83ED4-93AC-F047-AF73-BA3F105A6D0A}" name="start_time" dataDxfId="14"/>
-    <tableColumn id="2" xr3:uid="{F0229387-F330-284C-B4AE-1D5D5E6605D1}" name="end_time" dataDxfId="13"/>
-    <tableColumn id="3" xr3:uid="{FEBDECC5-2779-A649-A021-31F708F52761}" name="time_diff" dataDxfId="12">
+    <tableColumn id="1" xr3:uid="{25E83ED4-93AC-F047-AF73-BA3F105A6D0A}" name="start_time" dataDxfId="20"/>
+    <tableColumn id="2" xr3:uid="{F0229387-F330-284C-B4AE-1D5D5E6605D1}" name="end_time" dataDxfId="19"/>
+    <tableColumn id="3" xr3:uid="{FEBDECC5-2779-A649-A021-31F708F52761}" name="time_diff" dataDxfId="18">
       <calculatedColumnFormula>Table245152122[[#This Row],[end_time]]-Table245152122[[#This Row],[start_time]]</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="4" xr3:uid="{AF082110-2951-F84E-8D3A-9165E0C2C148}" name="notes"/>
@@ -1458,9 +1496,9 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="28" xr:uid="{661D3210-775C-8040-8FE5-26CDF0E1C0C6}" name="Table2451529" displayName="Table2451529" ref="A1:D31" totalsRowShown="0">
   <autoFilter ref="A1:D31" xr:uid="{1A93302E-8621-7D48-88F2-5AC51E7EA3A4}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{ED768153-5408-0040-8E27-7A60AC8E2998}" name="start_time" dataDxfId="11"/>
-    <tableColumn id="2" xr3:uid="{85BF026F-4EF2-414B-97C8-8F4A405735DA}" name="end_time" dataDxfId="10"/>
-    <tableColumn id="3" xr3:uid="{FA7B9F4D-D773-3944-A5EF-C6BF952DF273}" name="time_diff" dataDxfId="9">
+    <tableColumn id="1" xr3:uid="{ED768153-5408-0040-8E27-7A60AC8E2998}" name="start_time" dataDxfId="17"/>
+    <tableColumn id="2" xr3:uid="{85BF026F-4EF2-414B-97C8-8F4A405735DA}" name="end_time" dataDxfId="16"/>
+    <tableColumn id="3" xr3:uid="{FA7B9F4D-D773-3944-A5EF-C6BF952DF273}" name="time_diff" dataDxfId="15">
       <calculatedColumnFormula>Table2451529[[#This Row],[end_time]]-Table2451529[[#This Row],[start_time]]</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="4" xr3:uid="{93ED54FD-B021-8042-8A26-06CABF9E31ED}" name="notes"/>
@@ -1473,9 +1511,9 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="29" xr:uid="{2A32B478-DE8E-8744-8E1D-E79CAB721CFA}" name="Table245152930" displayName="Table245152930" ref="A1:D31" totalsRowShown="0">
   <autoFilter ref="A1:D31" xr:uid="{1A93302E-8621-7D48-88F2-5AC51E7EA3A4}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{79880ACD-2F16-8B41-B96B-06D8373CF56F}" name="start_time" dataDxfId="8"/>
-    <tableColumn id="2" xr3:uid="{5EBA4F35-D0D6-5841-8642-F7EB935C9D15}" name="end_time" dataDxfId="7"/>
-    <tableColumn id="3" xr3:uid="{33ADB2D4-D36E-C540-B4EE-1777AB5350B0}" name="time_diff" dataDxfId="6">
+    <tableColumn id="1" xr3:uid="{79880ACD-2F16-8B41-B96B-06D8373CF56F}" name="start_time" dataDxfId="14"/>
+    <tableColumn id="2" xr3:uid="{5EBA4F35-D0D6-5841-8642-F7EB935C9D15}" name="end_time" dataDxfId="13"/>
+    <tableColumn id="3" xr3:uid="{33ADB2D4-D36E-C540-B4EE-1777AB5350B0}" name="time_diff" dataDxfId="12">
       <calculatedColumnFormula>Table245152930[[#This Row],[end_time]]-Table245152930[[#This Row],[start_time]]</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="4" xr3:uid="{67846232-3E2C-AF45-BD20-49FA08924520}" name="notes"/>
@@ -1490,7 +1528,7 @@
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{01F56379-480D-E144-8844-79E29F338160}" name="start_time"/>
     <tableColumn id="2" xr3:uid="{80A1EC3F-97BF-2A42-A823-A672AD58C802}" name="end_time"/>
-    <tableColumn id="3" xr3:uid="{F529491E-B189-F14F-8D98-A6DD0470EB40}" name="time_diff" dataDxfId="80">
+    <tableColumn id="3" xr3:uid="{F529491E-B189-F14F-8D98-A6DD0470EB40}" name="time_diff" dataDxfId="86">
       <calculatedColumnFormula>Table2[[#This Row],[end_time]]-Table2[[#This Row],[start_time]]</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="4" xr3:uid="{DC0F7FFE-563B-3E40-AAB4-A68B98253F92}" name="notes"/>
@@ -1503,9 +1541,9 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="30" xr:uid="{2EB2F573-CED5-AA4A-8CF8-F3AEF0AA7723}" name="Table245152931" displayName="Table245152931" ref="A1:D31" totalsRowShown="0">
   <autoFilter ref="A1:D31" xr:uid="{1A93302E-8621-7D48-88F2-5AC51E7EA3A4}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{73DC15AF-3DAA-8143-AF82-F1D507DCE96F}" name="start_time" dataDxfId="5"/>
-    <tableColumn id="2" xr3:uid="{D5FE6EE4-7C86-FF49-BF49-4BE6F39FC1A9}" name="end_time" dataDxfId="4"/>
-    <tableColumn id="3" xr3:uid="{19EF1AAC-C504-8E46-AE44-B9439BD37567}" name="time_diff" dataDxfId="3">
+    <tableColumn id="1" xr3:uid="{73DC15AF-3DAA-8143-AF82-F1D507DCE96F}" name="start_time" dataDxfId="11"/>
+    <tableColumn id="2" xr3:uid="{D5FE6EE4-7C86-FF49-BF49-4BE6F39FC1A9}" name="end_time" dataDxfId="10"/>
+    <tableColumn id="3" xr3:uid="{19EF1AAC-C504-8E46-AE44-B9439BD37567}" name="time_diff" dataDxfId="9">
       <calculatedColumnFormula>Table245152931[[#This Row],[end_time]]-Table245152931[[#This Row],[start_time]]</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="4" xr3:uid="{00B18BD3-325E-1D4C-918C-B906E01F9629}" name="notes"/>
@@ -1518,12 +1556,42 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="31" xr:uid="{199CB066-B051-3341-ADBB-1E54C19CADA1}" name="Table24515293132" displayName="Table24515293132" ref="A1:D31" totalsRowShown="0">
   <autoFilter ref="A1:D31" xr:uid="{1A93302E-8621-7D48-88F2-5AC51E7EA3A4}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{2A4F6AEE-4765-4041-B244-0BEE39578BB0}" name="start_time" dataDxfId="2"/>
-    <tableColumn id="2" xr3:uid="{860B172B-36D9-6C40-AEBE-E23FD467A8C3}" name="end_time" dataDxfId="1"/>
-    <tableColumn id="3" xr3:uid="{2F5A21E2-41C6-384E-ACA1-907DDE787D4B}" name="time_diff" dataDxfId="0">
+    <tableColumn id="1" xr3:uid="{2A4F6AEE-4765-4041-B244-0BEE39578BB0}" name="start_time" dataDxfId="8"/>
+    <tableColumn id="2" xr3:uid="{860B172B-36D9-6C40-AEBE-E23FD467A8C3}" name="end_time" dataDxfId="7"/>
+    <tableColumn id="3" xr3:uid="{2F5A21E2-41C6-384E-ACA1-907DDE787D4B}" name="time_diff" dataDxfId="6">
       <calculatedColumnFormula>Table24515293132[[#This Row],[end_time]]-Table24515293132[[#This Row],[start_time]]</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="4" xr3:uid="{0DC69275-E5B9-2141-B9B8-C11748283861}" name="notes"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table32.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="32" xr:uid="{06A6F3E2-626F-8B4A-9E0D-9700F934709A}" name="Table2451533" displayName="Table2451533" ref="A1:D31" totalsRowShown="0">
+  <autoFilter ref="A1:D31" xr:uid="{1A93302E-8621-7D48-88F2-5AC51E7EA3A4}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{6F3BA02B-C7C3-3648-AEF6-CE3B7B5C96AE}" name="start_time" dataDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{EB6C5B05-913E-6C4F-8330-3E7CBDBA2766}" name="end_time" dataDxfId="4"/>
+    <tableColumn id="3" xr3:uid="{21CEE3A7-1FA0-5749-9CC4-B7EF3AEBA3F9}" name="time_diff" dataDxfId="3">
+      <calculatedColumnFormula>Table2451533[[#This Row],[end_time]]-Table2451533[[#This Row],[start_time]]</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="4" xr3:uid="{0DB42EF9-5D80-2145-8D74-E69681387C37}" name="notes"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table33.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="33" xr:uid="{3A4EBCD4-7107-744D-876A-39BF783E4518}" name="Table245153334" displayName="Table245153334" ref="A1:D31" totalsRowShown="0">
+  <autoFilter ref="A1:D31" xr:uid="{1A93302E-8621-7D48-88F2-5AC51E7EA3A4}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{2EF55489-2CD2-374A-A411-45BFC6EF0F11}" name="start_time" dataDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{3A3B2D6B-229B-534D-913B-CD67E99E2FC0}" name="end_time" dataDxfId="1"/>
+    <tableColumn id="3" xr3:uid="{1582DACA-6910-E747-AC0A-911487FD8F40}" name="time_diff" dataDxfId="0">
+      <calculatedColumnFormula>Table245153334[[#This Row],[end_time]]-Table245153334[[#This Row],[start_time]]</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="4" xr3:uid="{3964B772-35E4-B248-AE1D-C3E807B80CB1}" name="notes"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1535,7 +1603,7 @@
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{7197966F-DB73-A94E-B2AE-FF5E410916CA}" name="start_time"/>
     <tableColumn id="2" xr3:uid="{615965FE-9104-054A-86EF-13FD1960F3F6}" name="end_time"/>
-    <tableColumn id="3" xr3:uid="{B0854C19-C681-7640-AAB6-06872F731D13}" name="time_diff" dataDxfId="79">
+    <tableColumn id="3" xr3:uid="{B0854C19-C681-7640-AAB6-06872F731D13}" name="time_diff" dataDxfId="85">
       <calculatedColumnFormula>Table213[[#This Row],[end_time]]-Table213[[#This Row],[start_time]]</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="4" xr3:uid="{0469E901-54FA-974D-A28F-40EC1AA491CD}" name="notes"/>
@@ -1548,9 +1616,9 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{DAC55445-B449-1B46-ADAD-5D1EE6A1BD3D}" name="Table246" displayName="Table246" ref="A1:D31" totalsRowShown="0">
   <autoFilter ref="A1:D31" xr:uid="{7DCBAB66-89F8-6F47-8D64-FA0C26924201}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{54C1AFBA-849B-564E-9383-040E585C368C}" name="start_time" dataDxfId="78"/>
-    <tableColumn id="2" xr3:uid="{45F9645E-00F2-4A47-AB06-DBB721851807}" name="end_time" dataDxfId="77"/>
-    <tableColumn id="3" xr3:uid="{D8F0A3A2-BBC5-6D49-8527-799E99BCFA49}" name="time_diff" dataDxfId="76">
+    <tableColumn id="1" xr3:uid="{54C1AFBA-849B-564E-9383-040E585C368C}" name="start_time" dataDxfId="84"/>
+    <tableColumn id="2" xr3:uid="{45F9645E-00F2-4A47-AB06-DBB721851807}" name="end_time" dataDxfId="83"/>
+    <tableColumn id="3" xr3:uid="{D8F0A3A2-BBC5-6D49-8527-799E99BCFA49}" name="time_diff" dataDxfId="82">
       <calculatedColumnFormula>Table246[[#This Row],[end_time]]-Table246[[#This Row],[start_time]]</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="4" xr3:uid="{838825F0-239B-C440-9C0B-3A9D1E9C0D95}" name="notes"/>
@@ -1565,7 +1633,7 @@
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{97B35572-DA30-684F-B3E5-729DB08045CE}" name="start_time"/>
     <tableColumn id="2" xr3:uid="{CB979489-F330-CB47-ACD8-45591E7E6177}" name="end_time"/>
-    <tableColumn id="3" xr3:uid="{C2A1FF6A-8B35-0348-85B8-BCECB7F2BCFE}" name="time_diff" dataDxfId="75">
+    <tableColumn id="3" xr3:uid="{C2A1FF6A-8B35-0348-85B8-BCECB7F2BCFE}" name="time_diff" dataDxfId="81">
       <calculatedColumnFormula>Table21314[[#This Row],[end_time]]-Table21314[[#This Row],[start_time]]</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="4" xr3:uid="{C144438C-DE22-7644-A5DB-5310B9F06FD7}" name="notes"/>
@@ -1578,9 +1646,9 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="22" xr:uid="{BB18B32E-8D1B-4E40-800B-981F430F8CDD}" name="Table24515345678" displayName="Table24515345678" ref="A1:D31" totalsRowShown="0">
   <autoFilter ref="A1:D31" xr:uid="{1A93302E-8621-7D48-88F2-5AC51E7EA3A4}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{9D16D395-E4E3-DB45-90F5-E5327318AF10}" name="start_time" dataDxfId="74"/>
-    <tableColumn id="2" xr3:uid="{6060AEBF-3E3A-5A47-BE28-82B21D4A9A71}" name="end_time" dataDxfId="73"/>
-    <tableColumn id="3" xr3:uid="{B44166A9-5F8E-0847-90D8-CD1B96CFFCBD}" name="time_diff" dataDxfId="72">
+    <tableColumn id="1" xr3:uid="{9D16D395-E4E3-DB45-90F5-E5327318AF10}" name="start_time" dataDxfId="80"/>
+    <tableColumn id="2" xr3:uid="{6060AEBF-3E3A-5A47-BE28-82B21D4A9A71}" name="end_time" dataDxfId="79"/>
+    <tableColumn id="3" xr3:uid="{B44166A9-5F8E-0847-90D8-CD1B96CFFCBD}" name="time_diff" dataDxfId="78">
       <calculatedColumnFormula>Table24515345678[[#This Row],[end_time]]-Table24515345678[[#This Row],[start_time]]</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="4" xr3:uid="{622F2CC9-1E07-0745-BD46-0FF8E04F606C}" name="notes"/>
@@ -1593,9 +1661,9 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="23" xr:uid="{C3F9313B-C284-1146-B033-93DD207396CF}" name="Table2451534567" displayName="Table2451534567" ref="A1:D31" totalsRowShown="0">
   <autoFilter ref="A1:D31" xr:uid="{1A93302E-8621-7D48-88F2-5AC51E7EA3A4}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{C2F60EB9-3A21-F943-85B0-6892CFC0EFE9}" name="start_time" dataDxfId="71"/>
-    <tableColumn id="2" xr3:uid="{B9B7F5F7-DC74-FC4D-8DE1-ABE02D48F190}" name="end_time" dataDxfId="70"/>
-    <tableColumn id="3" xr3:uid="{EBD1F883-E2BA-6049-9C36-BA4E73D36AAC}" name="time_diff" dataDxfId="69">
+    <tableColumn id="1" xr3:uid="{C2F60EB9-3A21-F943-85B0-6892CFC0EFE9}" name="start_time" dataDxfId="77"/>
+    <tableColumn id="2" xr3:uid="{B9B7F5F7-DC74-FC4D-8DE1-ABE02D48F190}" name="end_time" dataDxfId="76"/>
+    <tableColumn id="3" xr3:uid="{EBD1F883-E2BA-6049-9C36-BA4E73D36AAC}" name="time_diff" dataDxfId="75">
       <calculatedColumnFormula>Table2451534567[[#This Row],[end_time]]-Table2451534567[[#This Row],[start_time]]</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="4" xr3:uid="{9BD53916-30AA-4E4F-989F-570ACDB86B60}" name="notes"/>
@@ -1608,9 +1676,9 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{C7DEA103-B67A-0B49-99E5-BEE70970D4BB}" name="Table247" displayName="Table247" ref="A1:D31" totalsRowShown="0">
   <autoFilter ref="A1:D31" xr:uid="{7DCBAB66-89F8-6F47-8D64-FA0C26924201}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{CB152735-EDBE-5144-8A33-370189AD9329}" name="start_time" dataDxfId="68"/>
-    <tableColumn id="2" xr3:uid="{78FDD20A-A666-E94B-A38C-0886D5E9FD55}" name="end_time" dataDxfId="67"/>
-    <tableColumn id="3" xr3:uid="{AE363FE2-700D-BC49-BD68-6E6DB6F05C17}" name="time_diff" dataDxfId="66">
+    <tableColumn id="1" xr3:uid="{CB152735-EDBE-5144-8A33-370189AD9329}" name="start_time" dataDxfId="74"/>
+    <tableColumn id="2" xr3:uid="{78FDD20A-A666-E94B-A38C-0886D5E9FD55}" name="end_time" dataDxfId="73"/>
+    <tableColumn id="3" xr3:uid="{AE363FE2-700D-BC49-BD68-6E6DB6F05C17}" name="time_diff" dataDxfId="72">
       <calculatedColumnFormula>Table247[[#This Row],[end_time]]-Table247[[#This Row],[start_time]]</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="4" xr3:uid="{CCA0740F-5707-C44E-AA57-B44DAE132805}" name="notes"/>
@@ -7749,8 +7817,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8F4A8F4-AAF9-534C-A76C-45D54A4AA321}">
   <dimension ref="A1:G43"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B1048576"/>
+    <sheetView zoomScale="125" workbookViewId="0">
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8322,11 +8390,33 @@
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A29" s="1"/>
+      <c r="A29" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="D29" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="E29" s="6" t="s">
+        <v>69</v>
+      </c>
       <c r="F29" s="2"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A30" s="1"/>
+      <c r="A30" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="B30" s="6">
+        <v>1414</v>
+      </c>
+      <c r="C30" s="6">
+        <v>2064</v>
+      </c>
+      <c r="D30" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="E30" s="6" t="s">
+        <v>69</v>
+      </c>
       <c r="F30" s="2"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.2">
@@ -15117,6 +15207,1116 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68F00F07-6F7D-BC4B-9E0C-BCAADD61651A}">
+  <dimension ref="A1:I41"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="4" max="4" width="72.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="H1" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="I1" s="13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A2" s="5"/>
+      <c r="B2" s="5"/>
+      <c r="C2" s="4">
+        <f>Table2451533[[#This Row],[end_time]]-Table2451533[[#This Row],[start_time]]</f>
+        <v>0</v>
+      </c>
+      <c r="F2" s="14"/>
+      <c r="G2" s="14"/>
+      <c r="H2" s="14">
+        <f>G2-F2</f>
+        <v>0</v>
+      </c>
+      <c r="I2" s="15"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A3" s="5"/>
+      <c r="B3" s="5"/>
+      <c r="C3" s="4">
+        <f>Table2451533[[#This Row],[end_time]]-Table2451533[[#This Row],[start_time]]</f>
+        <v>0</v>
+      </c>
+      <c r="F3" s="16"/>
+      <c r="G3" s="16"/>
+      <c r="H3" s="16">
+        <f>G3-F3</f>
+        <v>0</v>
+      </c>
+      <c r="I3" s="11"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A4" s="5"/>
+      <c r="B4" s="5"/>
+      <c r="C4" s="4">
+        <f>Table2451533[[#This Row],[end_time]]-Table2451533[[#This Row],[start_time]]</f>
+        <v>0</v>
+      </c>
+      <c r="F4" s="14"/>
+      <c r="G4" s="14"/>
+      <c r="H4" s="14">
+        <f t="shared" ref="H4:H31" si="0">G4-F4</f>
+        <v>0</v>
+      </c>
+      <c r="I4" s="15"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A5" s="5"/>
+      <c r="B5" s="5"/>
+      <c r="C5" s="4">
+        <f>Table2451533[[#This Row],[end_time]]-Table2451533[[#This Row],[start_time]]</f>
+        <v>0</v>
+      </c>
+      <c r="F5" s="16"/>
+      <c r="G5" s="16"/>
+      <c r="H5" s="16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I5" s="11"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A6" s="5"/>
+      <c r="B6" s="5"/>
+      <c r="C6" s="4">
+        <f>Table2451533[[#This Row],[end_time]]-Table2451533[[#This Row],[start_time]]</f>
+        <v>0</v>
+      </c>
+      <c r="F6" s="14"/>
+      <c r="G6" s="14"/>
+      <c r="H6" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I6" s="15"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A7" s="5"/>
+      <c r="B7" s="5"/>
+      <c r="C7" s="4">
+        <f>Table2451533[[#This Row],[end_time]]-Table2451533[[#This Row],[start_time]]</f>
+        <v>0</v>
+      </c>
+      <c r="F7" s="16"/>
+      <c r="G7" s="16"/>
+      <c r="H7" s="16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I7" s="11"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A8" s="5"/>
+      <c r="B8" s="5"/>
+      <c r="C8" s="4">
+        <f>Table2451533[[#This Row],[end_time]]-Table2451533[[#This Row],[start_time]]</f>
+        <v>0</v>
+      </c>
+      <c r="F8" s="15"/>
+      <c r="G8" s="15"/>
+      <c r="H8" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I8" s="15"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A9" s="5"/>
+      <c r="B9" s="5"/>
+      <c r="C9" s="4">
+        <f>Table2451533[[#This Row],[end_time]]-Table2451533[[#This Row],[start_time]]</f>
+        <v>0</v>
+      </c>
+      <c r="F9" s="11"/>
+      <c r="G9" s="11"/>
+      <c r="H9" s="16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I9" s="11"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A10" s="5"/>
+      <c r="B10" s="5"/>
+      <c r="C10" s="4">
+        <f>Table2451533[[#This Row],[end_time]]-Table2451533[[#This Row],[start_time]]</f>
+        <v>0</v>
+      </c>
+      <c r="F10" s="15"/>
+      <c r="G10" s="15"/>
+      <c r="H10" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I10" s="15"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A11" s="5"/>
+      <c r="B11" s="5"/>
+      <c r="C11" s="4">
+        <f>Table2451533[[#This Row],[end_time]]-Table2451533[[#This Row],[start_time]]</f>
+        <v>0</v>
+      </c>
+      <c r="F11" s="11"/>
+      <c r="G11" s="11"/>
+      <c r="H11" s="16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I11" s="11"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A12" s="5"/>
+      <c r="B12" s="5"/>
+      <c r="C12" s="4">
+        <f>Table2451533[[#This Row],[end_time]]-Table2451533[[#This Row],[start_time]]</f>
+        <v>0</v>
+      </c>
+      <c r="F12" s="15"/>
+      <c r="G12" s="15"/>
+      <c r="H12" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I12" s="15"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A13" s="5"/>
+      <c r="B13" s="5"/>
+      <c r="C13" s="4">
+        <f>Table2451533[[#This Row],[end_time]]-Table2451533[[#This Row],[start_time]]</f>
+        <v>0</v>
+      </c>
+      <c r="F13" s="11"/>
+      <c r="G13" s="11"/>
+      <c r="H13" s="16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I13" s="11"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A14" s="5"/>
+      <c r="B14" s="5"/>
+      <c r="C14" s="4">
+        <f>Table2451533[[#This Row],[end_time]]-Table2451533[[#This Row],[start_time]]</f>
+        <v>0</v>
+      </c>
+      <c r="F14" s="15"/>
+      <c r="G14" s="15"/>
+      <c r="H14" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I14" s="15"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A15" s="5"/>
+      <c r="B15" s="5"/>
+      <c r="C15" s="4">
+        <f>Table2451533[[#This Row],[end_time]]-Table2451533[[#This Row],[start_time]]</f>
+        <v>0</v>
+      </c>
+      <c r="F15" s="11"/>
+      <c r="G15" s="11"/>
+      <c r="H15" s="16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I15" s="11"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A16" s="5"/>
+      <c r="B16" s="5"/>
+      <c r="C16" s="4">
+        <f>Table2451533[[#This Row],[end_time]]-Table2451533[[#This Row],[start_time]]</f>
+        <v>0</v>
+      </c>
+      <c r="F16" s="15"/>
+      <c r="G16" s="15"/>
+      <c r="H16" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I16" s="15"/>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A17" s="5"/>
+      <c r="B17" s="5"/>
+      <c r="C17" s="4">
+        <f>Table2451533[[#This Row],[end_time]]-Table2451533[[#This Row],[start_time]]</f>
+        <v>0</v>
+      </c>
+      <c r="F17" s="11"/>
+      <c r="G17" s="11"/>
+      <c r="H17" s="16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I17" s="11"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A18" s="5"/>
+      <c r="B18" s="5"/>
+      <c r="C18" s="4">
+        <f>Table2451533[[#This Row],[end_time]]-Table2451533[[#This Row],[start_time]]</f>
+        <v>0</v>
+      </c>
+      <c r="F18" s="15"/>
+      <c r="G18" s="15"/>
+      <c r="H18" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I18" s="15"/>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A19" s="5"/>
+      <c r="B19" s="5"/>
+      <c r="C19" s="4">
+        <f>Table2451533[[#This Row],[end_time]]-Table2451533[[#This Row],[start_time]]</f>
+        <v>0</v>
+      </c>
+      <c r="F19" s="11"/>
+      <c r="G19" s="11"/>
+      <c r="H19" s="16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I19" s="11"/>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A20" s="5"/>
+      <c r="B20" s="5"/>
+      <c r="C20" s="4">
+        <f>Table2451533[[#This Row],[end_time]]-Table2451533[[#This Row],[start_time]]</f>
+        <v>0</v>
+      </c>
+      <c r="F20" s="15"/>
+      <c r="G20" s="15"/>
+      <c r="H20" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I20" s="15"/>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A21" s="5"/>
+      <c r="B21" s="5"/>
+      <c r="C21" s="4">
+        <f>Table2451533[[#This Row],[end_time]]-Table2451533[[#This Row],[start_time]]</f>
+        <v>0</v>
+      </c>
+      <c r="F21" s="11"/>
+      <c r="G21" s="11"/>
+      <c r="H21" s="16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I21" s="11"/>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A22" s="5"/>
+      <c r="B22" s="5"/>
+      <c r="C22" s="4">
+        <f>Table2451533[[#This Row],[end_time]]-Table2451533[[#This Row],[start_time]]</f>
+        <v>0</v>
+      </c>
+      <c r="F22" s="15"/>
+      <c r="G22" s="15"/>
+      <c r="H22" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I22" s="15"/>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A23" s="5"/>
+      <c r="B23" s="5"/>
+      <c r="C23" s="4">
+        <f>Table2451533[[#This Row],[end_time]]-Table2451533[[#This Row],[start_time]]</f>
+        <v>0</v>
+      </c>
+      <c r="F23" s="11"/>
+      <c r="G23" s="11"/>
+      <c r="H23" s="16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I23" s="11"/>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A24" s="5"/>
+      <c r="B24" s="5"/>
+      <c r="C24" s="4">
+        <f>Table2451533[[#This Row],[end_time]]-Table2451533[[#This Row],[start_time]]</f>
+        <v>0</v>
+      </c>
+      <c r="F24" s="15"/>
+      <c r="G24" s="15"/>
+      <c r="H24" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I24" s="15"/>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A25" s="5"/>
+      <c r="B25" s="5"/>
+      <c r="C25" s="4">
+        <f>Table2451533[[#This Row],[end_time]]-Table2451533[[#This Row],[start_time]]</f>
+        <v>0</v>
+      </c>
+      <c r="F25" s="11"/>
+      <c r="G25" s="11"/>
+      <c r="H25" s="16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I25" s="11"/>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A26" s="5"/>
+      <c r="B26" s="5"/>
+      <c r="C26" s="4">
+        <f>Table2451533[[#This Row],[end_time]]-Table2451533[[#This Row],[start_time]]</f>
+        <v>0</v>
+      </c>
+      <c r="F26" s="15"/>
+      <c r="G26" s="15"/>
+      <c r="H26" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I26" s="15"/>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A27" s="5"/>
+      <c r="B27" s="5"/>
+      <c r="C27" s="4">
+        <f>Table2451533[[#This Row],[end_time]]-Table2451533[[#This Row],[start_time]]</f>
+        <v>0</v>
+      </c>
+      <c r="F27" s="11"/>
+      <c r="G27" s="11"/>
+      <c r="H27" s="16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I27" s="11"/>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A28" s="5"/>
+      <c r="B28" s="5"/>
+      <c r="C28" s="4">
+        <f>Table2451533[[#This Row],[end_time]]-Table2451533[[#This Row],[start_time]]</f>
+        <v>0</v>
+      </c>
+      <c r="F28" s="15"/>
+      <c r="G28" s="15"/>
+      <c r="H28" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I28" s="15"/>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A29" s="5"/>
+      <c r="B29" s="5"/>
+      <c r="C29" s="4">
+        <f>Table2451533[[#This Row],[end_time]]-Table2451533[[#This Row],[start_time]]</f>
+        <v>0</v>
+      </c>
+      <c r="F29" s="11"/>
+      <c r="G29" s="11"/>
+      <c r="H29" s="16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I29" s="11"/>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A30" s="5"/>
+      <c r="B30" s="5"/>
+      <c r="C30" s="4">
+        <f>Table2451533[[#This Row],[end_time]]-Table2451533[[#This Row],[start_time]]</f>
+        <v>0</v>
+      </c>
+      <c r="F30" s="15"/>
+      <c r="G30" s="15"/>
+      <c r="H30" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I30" s="15"/>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A31" s="5"/>
+      <c r="B31" s="5"/>
+      <c r="C31" s="4">
+        <f>Table2451533[[#This Row],[end_time]]-Table2451533[[#This Row],[start_time]]</f>
+        <v>0</v>
+      </c>
+      <c r="F31" s="17"/>
+      <c r="G31" s="17"/>
+      <c r="H31" s="20">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I31" s="17"/>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="E32" s="2"/>
+      <c r="F32" s="11"/>
+      <c r="G32" s="11"/>
+      <c r="H32" s="11"/>
+      <c r="I32" s="11"/>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>52</v>
+      </c>
+      <c r="C33" s="6">
+        <f>HOUR(SUM(Table2451533[time_diff]))*3600 + MINUTE(SUM(Table2451533[time_diff])) * 60 + SECOND(SUM(Table2451533[time_diff]))</f>
+        <v>0</v>
+      </c>
+      <c r="F33" s="11" t="s">
+        <v>87</v>
+      </c>
+      <c r="G33" s="11"/>
+      <c r="H33" s="6">
+        <f>HOUR(SUM(H2:H31))*3600 + MINUTE(SUM(H2:H31)) * 60 + SECOND(SUM(H2:H31))</f>
+        <v>0</v>
+      </c>
+      <c r="I33" s="11"/>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="C34" s="4"/>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="C35" s="5"/>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="C36" s="5"/>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="C37" s="6"/>
+      <c r="E37" s="6"/>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="D41" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{420C3755-3FEC-2044-A90C-C2D3BB18642F}">
+  <dimension ref="A1:I41"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I5" sqref="I5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="4" max="4" width="72.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="H1" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="I1" s="13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A2" s="5">
+        <v>0.47834490740740743</v>
+      </c>
+      <c r="B2" s="5">
+        <v>0.48207175925925927</v>
+      </c>
+      <c r="C2" s="4">
+        <f>Table245153334[[#This Row],[end_time]]-Table245153334[[#This Row],[start_time]]</f>
+        <v>3.7268518518518423E-3</v>
+      </c>
+      <c r="F2" s="14">
+        <v>0.4755671296296296</v>
+      </c>
+      <c r="G2" s="14">
+        <v>0.48466435185185186</v>
+      </c>
+      <c r="H2" s="14">
+        <f>G2-F2</f>
+        <v>9.0972222222222565E-3</v>
+      </c>
+      <c r="I2" s="15" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A3" s="5">
+        <v>0.48743055555555553</v>
+      </c>
+      <c r="B3" s="5">
+        <v>0.49681712962962965</v>
+      </c>
+      <c r="C3" s="4">
+        <f>Table245153334[[#This Row],[end_time]]-Table245153334[[#This Row],[start_time]]</f>
+        <v>9.3865740740741166E-3</v>
+      </c>
+      <c r="D3" t="s">
+        <v>167</v>
+      </c>
+      <c r="F3" s="16">
+        <v>0.48652777777777778</v>
+      </c>
+      <c r="G3" s="16">
+        <v>0.4971990740740741</v>
+      </c>
+      <c r="H3" s="16">
+        <f>G3-F3</f>
+        <v>1.0671296296296318E-2</v>
+      </c>
+      <c r="I3" s="11"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A4" s="5">
+        <v>0.50685185185185189</v>
+      </c>
+      <c r="B4" s="5">
+        <v>0.51010416666666669</v>
+      </c>
+      <c r="C4" s="4">
+        <f>Table245153334[[#This Row],[end_time]]-Table245153334[[#This Row],[start_time]]</f>
+        <v>3.2523148148148051E-3</v>
+      </c>
+      <c r="D4" t="s">
+        <v>168</v>
+      </c>
+      <c r="F4" s="14">
+        <v>0.50609953703703703</v>
+      </c>
+      <c r="G4" s="14">
+        <v>0.51021990740740741</v>
+      </c>
+      <c r="H4" s="14">
+        <f t="shared" ref="H4:H31" si="0">G4-F4</f>
+        <v>4.1203703703703853E-3</v>
+      </c>
+      <c r="I4" s="15" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A5" s="5"/>
+      <c r="B5" s="5"/>
+      <c r="C5" s="4">
+        <f>Table245153334[[#This Row],[end_time]]-Table245153334[[#This Row],[start_time]]</f>
+        <v>0</v>
+      </c>
+      <c r="F5" s="16"/>
+      <c r="G5" s="16"/>
+      <c r="H5" s="16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I5" s="11"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A6" s="5"/>
+      <c r="B6" s="5"/>
+      <c r="C6" s="4">
+        <f>Table245153334[[#This Row],[end_time]]-Table245153334[[#This Row],[start_time]]</f>
+        <v>0</v>
+      </c>
+      <c r="F6" s="14"/>
+      <c r="G6" s="14"/>
+      <c r="H6" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I6" s="15"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A7" s="5"/>
+      <c r="B7" s="5"/>
+      <c r="C7" s="4">
+        <f>Table245153334[[#This Row],[end_time]]-Table245153334[[#This Row],[start_time]]</f>
+        <v>0</v>
+      </c>
+      <c r="F7" s="16"/>
+      <c r="G7" s="16"/>
+      <c r="H7" s="16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I7" s="11"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A8" s="5"/>
+      <c r="B8" s="5"/>
+      <c r="C8" s="4">
+        <f>Table245153334[[#This Row],[end_time]]-Table245153334[[#This Row],[start_time]]</f>
+        <v>0</v>
+      </c>
+      <c r="F8" s="15"/>
+      <c r="G8" s="15"/>
+      <c r="H8" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I8" s="15"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A9" s="5"/>
+      <c r="B9" s="5"/>
+      <c r="C9" s="4">
+        <f>Table245153334[[#This Row],[end_time]]-Table245153334[[#This Row],[start_time]]</f>
+        <v>0</v>
+      </c>
+      <c r="F9" s="11"/>
+      <c r="G9" s="11"/>
+      <c r="H9" s="16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I9" s="11"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A10" s="5"/>
+      <c r="B10" s="5"/>
+      <c r="C10" s="4">
+        <f>Table245153334[[#This Row],[end_time]]-Table245153334[[#This Row],[start_time]]</f>
+        <v>0</v>
+      </c>
+      <c r="F10" s="15"/>
+      <c r="G10" s="15"/>
+      <c r="H10" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I10" s="15"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A11" s="5"/>
+      <c r="B11" s="5"/>
+      <c r="C11" s="4">
+        <f>Table245153334[[#This Row],[end_time]]-Table245153334[[#This Row],[start_time]]</f>
+        <v>0</v>
+      </c>
+      <c r="F11" s="11"/>
+      <c r="G11" s="11"/>
+      <c r="H11" s="16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I11" s="11"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A12" s="5"/>
+      <c r="B12" s="5"/>
+      <c r="C12" s="4">
+        <f>Table245153334[[#This Row],[end_time]]-Table245153334[[#This Row],[start_time]]</f>
+        <v>0</v>
+      </c>
+      <c r="F12" s="15"/>
+      <c r="G12" s="15"/>
+      <c r="H12" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I12" s="15"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A13" s="5"/>
+      <c r="B13" s="5"/>
+      <c r="C13" s="4">
+        <f>Table245153334[[#This Row],[end_time]]-Table245153334[[#This Row],[start_time]]</f>
+        <v>0</v>
+      </c>
+      <c r="F13" s="11"/>
+      <c r="G13" s="11"/>
+      <c r="H13" s="16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I13" s="11"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A14" s="5"/>
+      <c r="B14" s="5"/>
+      <c r="C14" s="4">
+        <f>Table245153334[[#This Row],[end_time]]-Table245153334[[#This Row],[start_time]]</f>
+        <v>0</v>
+      </c>
+      <c r="F14" s="15"/>
+      <c r="G14" s="15"/>
+      <c r="H14" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I14" s="15"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A15" s="5"/>
+      <c r="B15" s="5"/>
+      <c r="C15" s="4">
+        <f>Table245153334[[#This Row],[end_time]]-Table245153334[[#This Row],[start_time]]</f>
+        <v>0</v>
+      </c>
+      <c r="F15" s="11"/>
+      <c r="G15" s="11"/>
+      <c r="H15" s="16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I15" s="11"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A16" s="5"/>
+      <c r="B16" s="5"/>
+      <c r="C16" s="4">
+        <f>Table245153334[[#This Row],[end_time]]-Table245153334[[#This Row],[start_time]]</f>
+        <v>0</v>
+      </c>
+      <c r="F16" s="15"/>
+      <c r="G16" s="15"/>
+      <c r="H16" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I16" s="15"/>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A17" s="5"/>
+      <c r="B17" s="5"/>
+      <c r="C17" s="4">
+        <f>Table245153334[[#This Row],[end_time]]-Table245153334[[#This Row],[start_time]]</f>
+        <v>0</v>
+      </c>
+      <c r="F17" s="11"/>
+      <c r="G17" s="11"/>
+      <c r="H17" s="16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I17" s="11"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A18" s="5"/>
+      <c r="B18" s="5"/>
+      <c r="C18" s="4">
+        <f>Table245153334[[#This Row],[end_time]]-Table245153334[[#This Row],[start_time]]</f>
+        <v>0</v>
+      </c>
+      <c r="F18" s="15"/>
+      <c r="G18" s="15"/>
+      <c r="H18" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I18" s="15"/>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A19" s="5"/>
+      <c r="B19" s="5"/>
+      <c r="C19" s="4">
+        <f>Table245153334[[#This Row],[end_time]]-Table245153334[[#This Row],[start_time]]</f>
+        <v>0</v>
+      </c>
+      <c r="F19" s="11"/>
+      <c r="G19" s="11"/>
+      <c r="H19" s="16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I19" s="11"/>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A20" s="5"/>
+      <c r="B20" s="5"/>
+      <c r="C20" s="4">
+        <f>Table245153334[[#This Row],[end_time]]-Table245153334[[#This Row],[start_time]]</f>
+        <v>0</v>
+      </c>
+      <c r="F20" s="15"/>
+      <c r="G20" s="15"/>
+      <c r="H20" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I20" s="15"/>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A21" s="5"/>
+      <c r="B21" s="5"/>
+      <c r="C21" s="4">
+        <f>Table245153334[[#This Row],[end_time]]-Table245153334[[#This Row],[start_time]]</f>
+        <v>0</v>
+      </c>
+      <c r="F21" s="11"/>
+      <c r="G21" s="11"/>
+      <c r="H21" s="16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I21" s="11"/>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A22" s="5"/>
+      <c r="B22" s="5"/>
+      <c r="C22" s="4">
+        <f>Table245153334[[#This Row],[end_time]]-Table245153334[[#This Row],[start_time]]</f>
+        <v>0</v>
+      </c>
+      <c r="F22" s="15"/>
+      <c r="G22" s="15"/>
+      <c r="H22" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I22" s="15"/>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A23" s="5"/>
+      <c r="B23" s="5"/>
+      <c r="C23" s="4">
+        <f>Table245153334[[#This Row],[end_time]]-Table245153334[[#This Row],[start_time]]</f>
+        <v>0</v>
+      </c>
+      <c r="F23" s="11"/>
+      <c r="G23" s="11"/>
+      <c r="H23" s="16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I23" s="11"/>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A24" s="5"/>
+      <c r="B24" s="5"/>
+      <c r="C24" s="4">
+        <f>Table245153334[[#This Row],[end_time]]-Table245153334[[#This Row],[start_time]]</f>
+        <v>0</v>
+      </c>
+      <c r="F24" s="15"/>
+      <c r="G24" s="15"/>
+      <c r="H24" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I24" s="15"/>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A25" s="5"/>
+      <c r="B25" s="5"/>
+      <c r="C25" s="4">
+        <f>Table245153334[[#This Row],[end_time]]-Table245153334[[#This Row],[start_time]]</f>
+        <v>0</v>
+      </c>
+      <c r="F25" s="11"/>
+      <c r="G25" s="11"/>
+      <c r="H25" s="16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I25" s="11"/>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A26" s="5"/>
+      <c r="B26" s="5"/>
+      <c r="C26" s="4">
+        <f>Table245153334[[#This Row],[end_time]]-Table245153334[[#This Row],[start_time]]</f>
+        <v>0</v>
+      </c>
+      <c r="F26" s="15"/>
+      <c r="G26" s="15"/>
+      <c r="H26" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I26" s="15"/>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A27" s="5"/>
+      <c r="B27" s="5"/>
+      <c r="C27" s="4">
+        <f>Table245153334[[#This Row],[end_time]]-Table245153334[[#This Row],[start_time]]</f>
+        <v>0</v>
+      </c>
+      <c r="F27" s="11"/>
+      <c r="G27" s="11"/>
+      <c r="H27" s="16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I27" s="11"/>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A28" s="5"/>
+      <c r="B28" s="5"/>
+      <c r="C28" s="4">
+        <f>Table245153334[[#This Row],[end_time]]-Table245153334[[#This Row],[start_time]]</f>
+        <v>0</v>
+      </c>
+      <c r="F28" s="15"/>
+      <c r="G28" s="15"/>
+      <c r="H28" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I28" s="15"/>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A29" s="5"/>
+      <c r="B29" s="5"/>
+      <c r="C29" s="4">
+        <f>Table245153334[[#This Row],[end_time]]-Table245153334[[#This Row],[start_time]]</f>
+        <v>0</v>
+      </c>
+      <c r="F29" s="11"/>
+      <c r="G29" s="11"/>
+      <c r="H29" s="16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I29" s="11"/>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A30" s="5"/>
+      <c r="B30" s="5"/>
+      <c r="C30" s="4">
+        <f>Table245153334[[#This Row],[end_time]]-Table245153334[[#This Row],[start_time]]</f>
+        <v>0</v>
+      </c>
+      <c r="F30" s="15"/>
+      <c r="G30" s="15"/>
+      <c r="H30" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I30" s="15"/>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A31" s="5"/>
+      <c r="B31" s="5"/>
+      <c r="C31" s="4">
+        <f>Table245153334[[#This Row],[end_time]]-Table245153334[[#This Row],[start_time]]</f>
+        <v>0</v>
+      </c>
+      <c r="F31" s="17"/>
+      <c r="G31" s="17"/>
+      <c r="H31" s="20">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I31" s="17"/>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="E32" s="2"/>
+      <c r="F32" s="11"/>
+      <c r="G32" s="11"/>
+      <c r="H32" s="11"/>
+      <c r="I32" s="11"/>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>52</v>
+      </c>
+      <c r="C33" s="6">
+        <f>HOUR(SUM(Table245153334[time_diff]))*3600 + MINUTE(SUM(Table245153334[time_diff])) * 60 + SECOND(SUM(Table245153334[time_diff]))</f>
+        <v>1414</v>
+      </c>
+      <c r="F33" s="11" t="s">
+        <v>87</v>
+      </c>
+      <c r="G33" s="11"/>
+      <c r="H33" s="6">
+        <f>HOUR(SUM(H2:H31))*3600 + MINUTE(SUM(H2:H31)) * 60 + SECOND(SUM(H2:H31))</f>
+        <v>2064</v>
+      </c>
+      <c r="I33" s="11"/>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="C34" s="4"/>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="C35" s="5"/>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="C36" s="5"/>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="C37" s="6"/>
+      <c r="E37" s="6"/>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="D41" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B31B8D96-118F-A248-83C6-FD8A563415A9}">
   <dimension ref="A1:I37"/>
@@ -18152,6 +19352,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="3322fca5-43da-49d1-b081-466ee88b9b9d">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="08edd21d-9f77-405a-872a-1371c16ee465" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100BF6C17F5D6D98C42BF7485206F8FA016" ma:contentTypeVersion="15" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="d5edc83b350af0a5b53db876fcbb948f">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="3322fca5-43da-49d1-b081-466ee88b9b9d" xmlns:ns3="08edd21d-9f77-405a-872a-1371c16ee465" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="af4f449426634c4d4ecdf601b9961ca0" ns2:_="" ns3:_="">
     <xsd:import namespace="3322fca5-43da-49d1-b081-466ee88b9b9d"/>
@@ -18386,41 +19606,10 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="3322fca5-43da-49d1-b081-466ee88b9b9d">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="08edd21d-9f77-405a-872a-1371c16ee465" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B10E5675-4834-416E-A2AA-AFEE37EB2CC0}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{84C9AB0F-2376-4442-8FD0-7F9F6F9B731B}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="3322fca5-43da-49d1-b081-466ee88b9b9d"/>
-    <ds:schemaRef ds:uri="08edd21d-9f77-405a-872a-1371c16ee465"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -18443,9 +19632,20 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{84C9AB0F-2376-4442-8FD0-7F9F6F9B731B}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B10E5675-4834-416E-A2AA-AFEE37EB2CC0}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="3322fca5-43da-49d1-b081-466ee88b9b9d"/>
+    <ds:schemaRef ds:uri="08edd21d-9f77-405a-872a-1371c16ee465"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Add 1-024 and 1-025
</commit_message>
<xml_diff>
--- a/data/raw/VCAS-rove_time.xlsx
+++ b/data/raw/VCAS-rove_time.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10402"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10420"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jonathansalas/R_Projects/VCAS1_prelim_efficiency/data/raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2037EBE0-374E-A440-AB81-C9B4ECBE26BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93AF99F7-53C7-D442-A146-EB45CA999EC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="34560" windowHeight="21600" firstSheet="11" activeTab="31" xr2:uid="{0490BC07-0248-8949-839E-74C08EF47166}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="34560" windowHeight="21600" activeTab="1" xr2:uid="{0490BC07-0248-8949-839E-74C08EF47166}"/>
   </bookViews>
   <sheets>
     <sheet name="Notes" sheetId="1" r:id="rId1"/>
@@ -103,7 +103,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="570" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="572" uniqueCount="172">
   <si>
     <t>Here we track total ablation time which I will refer to going forward as rove_time</t>
   </si>
@@ -718,6 +718,12 @@
   </si>
   <si>
     <t>Done</t>
+  </si>
+  <si>
+    <t>https://fieldmedical.sharepoint.com/:v:/r/sites/Clinical/Shared%20Documents/VCAS%20Study/TMF-%20Subject%20Files/1-024/Footage/MIXoutput.mp4?csf=1&amp;web=1&amp;e=2sajXP</t>
+  </si>
+  <si>
+    <t>https://fieldmedical.sharepoint.com/:v:/r/sites/Clinical/Shared%20Documents/VCAS%20Study/TMF-%20Subject%20Files/1-025/Footage/mix.mp4?csf=1&amp;web=1&amp;e=pwO54g</t>
   </si>
 </sst>
 </file>
@@ -2020,7 +2026,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A535426F-7A8C-E949-810F-FB71A9FDBD02}">
   <dimension ref="A1:A36"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScale="161" workbookViewId="0">
+    <sheetView zoomScale="86" workbookViewId="0">
       <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
@@ -7817,8 +7823,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8F4A8F4-AAF9-534C-A76C-45D54A4AA321}">
   <dimension ref="A1:G43"/>
   <sheetViews>
-    <sheetView zoomScale="125" workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
+      <selection activeCell="F34" sqref="F34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8393,6 +8399,12 @@
       <c r="A29" s="1" t="s">
         <v>164</v>
       </c>
+      <c r="B29" s="6">
+        <v>2112</v>
+      </c>
+      <c r="C29" s="6">
+        <v>3775</v>
+      </c>
       <c r="D29" s="6" t="s">
         <v>98</v>
       </c>
@@ -8400,6 +8412,9 @@
         <v>69</v>
       </c>
       <c r="F29" s="2"/>
+      <c r="G29" s="3" t="s">
+        <v>170</v>
+      </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
@@ -8418,6 +8433,9 @@
         <v>69</v>
       </c>
       <c r="F30" s="2"/>
+      <c r="G30" s="3" t="s">
+        <v>171</v>
+      </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31" s="1"/>
@@ -8487,10 +8505,12 @@
     <hyperlink ref="G26" r:id="rId24" xr:uid="{4BB18C29-3E47-F944-B221-2FBC408E879F}"/>
     <hyperlink ref="G27" r:id="rId25" xr:uid="{D1899722-4A7F-C740-9D85-BB0987A5689C}"/>
     <hyperlink ref="G28" r:id="rId26" xr:uid="{238BB9F0-EE8E-7B41-B4BB-814C938F8075}"/>
+    <hyperlink ref="G29" r:id="rId27" xr:uid="{301FBC8D-1AA0-7E41-93E6-B959462BC5B5}"/>
+    <hyperlink ref="G30" r:id="rId28" xr:uid="{76D59AF6-DD10-5A43-8D8D-CB510BE93338}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
-    <tablePart r:id="rId27"/>
+    <tablePart r:id="rId29"/>
   </tableParts>
 </worksheet>
 </file>
@@ -15212,7 +15232,7 @@
   <dimension ref="A1:I41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="D39" sqref="D39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -15247,17 +15267,25 @@
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A2" s="5"/>
-      <c r="B2" s="5"/>
+      <c r="A2" s="5">
+        <v>0.46142361111111113</v>
+      </c>
+      <c r="B2" s="5">
+        <v>0.48586805555555557</v>
+      </c>
       <c r="C2" s="4">
         <f>Table2451533[[#This Row],[end_time]]-Table2451533[[#This Row],[start_time]]</f>
-        <v>0</v>
-      </c>
-      <c r="F2" s="14"/>
-      <c r="G2" s="14"/>
+        <v>2.4444444444444435E-2</v>
+      </c>
+      <c r="F2" s="14">
+        <v>0.45619212962962963</v>
+      </c>
+      <c r="G2" s="14">
+        <v>0.49988425925925928</v>
+      </c>
       <c r="H2" s="14">
         <f>G2-F2</f>
-        <v>0</v>
+        <v>4.369212962962965E-2</v>
       </c>
       <c r="I2" s="15"/>
     </row>
@@ -15709,7 +15737,7 @@
       </c>
       <c r="C33" s="6">
         <f>HOUR(SUM(Table2451533[time_diff]))*3600 + MINUTE(SUM(Table2451533[time_diff])) * 60 + SECOND(SUM(Table2451533[time_diff]))</f>
-        <v>0</v>
+        <v>2112</v>
       </c>
       <c r="F33" s="11" t="s">
         <v>87</v>
@@ -15717,7 +15745,7 @@
       <c r="G33" s="11"/>
       <c r="H33" s="6">
         <f>HOUR(SUM(H2:H31))*3600 + MINUTE(SUM(H2:H31)) * 60 + SECOND(SUM(H2:H31))</f>
-        <v>0</v>
+        <v>3775</v>
       </c>
       <c r="I33" s="11"/>
     </row>
@@ -15749,7 +15777,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{420C3755-3FEC-2044-A90C-C2D3BB18642F}">
   <dimension ref="A1:I41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
@@ -19352,15 +19380,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <lcf76f155ced4ddcb4097134ff3c332f xmlns="3322fca5-43da-49d1-b081-466ee88b9b9d">
@@ -19369,6 +19388,15 @@
     <TaxCatchAll xmlns="08edd21d-9f77-405a-872a-1371c16ee465" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -19607,14 +19635,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{84C9AB0F-2376-4442-8FD0-7F9F6F9B731B}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{711BD0AE-A67E-4DE0-BFB7-7F2D919E2D80}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
@@ -19627,6 +19647,14 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{84C9AB0F-2376-4442-8FD0-7F9F6F9B731B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Sent VCAS-I manuscript v1.5 on July 23rd with these code
</commit_message>
<xml_diff>
--- a/data/raw/VCAS-rove_time.xlsx
+++ b/data/raw/VCAS-rove_time.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10608"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jonathansalas/R_Projects/VCAS1_prelim_efficiency/data/raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A79AE96-8031-8845-A78B-6332E5128C1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8671877-AC2A-A547-BA6E-A4CC95B327E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="19940" activeTab="1" xr2:uid="{0490BC07-0248-8949-839E-74C08EF47166}"/>
   </bookViews>
@@ -2170,7 +2170,7 @@
   <dimension ref="A1:A36"/>
   <sheetViews>
     <sheetView zoomScale="86" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7966,8 +7966,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8F4A8F4-AAF9-534C-A76C-45D54A4AA321}">
   <dimension ref="A1:G43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="125" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="125" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -21789,6 +21789,17 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="3322fca5-43da-49d1-b081-466ee88b9b9d">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="08edd21d-9f77-405a-872a-1371c16ee465" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100BF6C17F5D6D98C42BF7485206F8FA016" ma:contentTypeVersion="15" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="d5edc83b350af0a5b53db876fcbb948f">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="3322fca5-43da-49d1-b081-466ee88b9b9d" xmlns:ns3="08edd21d-9f77-405a-872a-1371c16ee465" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="af4f449426634c4d4ecdf601b9961ca0" ns2:_="" ns3:_="">
     <xsd:import namespace="3322fca5-43da-49d1-b081-466ee88b9b9d"/>
@@ -22023,17 +22034,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="3322fca5-43da-49d1-b081-466ee88b9b9d">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="08edd21d-9f77-405a-872a-1371c16ee465" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{84C9AB0F-2376-4442-8FD0-7F9F6F9B731B}">
   <ds:schemaRefs>
@@ -22043,6 +22043,23 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{711BD0AE-A67E-4DE0-BFB7-7F2D919E2D80}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="08edd21d-9f77-405a-872a-1371c16ee465"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="3322fca5-43da-49d1-b081-466ee88b9b9d"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B10E5675-4834-416E-A2AA-AFEE37EB2CC0}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -22059,21 +22076,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{711BD0AE-A67E-4DE0-BFB7-7F2D919E2D80}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="08edd21d-9f77-405a-872a-1371c16ee465"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="3322fca5-43da-49d1-b081-466ee88b9b9d"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>